<commit_message>
Stabilize Phase G legacy compatibility and orchestrator flow
</commit_message>
<xml_diff>
--- a/data/AI_Talent_Landscape_Seed_Hubs.xlsx
+++ b/data/AI_Talent_Landscape_Seed_Hubs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davemendoza/Desktop/Research_First_Sourcer_Automation/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6822C7E4-21EE-244F-ACF7-780A54A283CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D2731802-4F3A-8A43-A005-570C85578FFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6720" yWindow="3800" windowWidth="51200" windowHeight="27060" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4440" yWindow="500" windowWidth="46540" windowHeight="27000" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PRIORITY_INDEX" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4751" uniqueCount="656">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4913" uniqueCount="674">
   <si>
     <t>Worksheet</t>
   </si>
@@ -2005,6 +2005,60 @@
   </si>
   <si>
     <t>weaviate</t>
+  </si>
+  <si>
+    <t>x6</t>
+  </si>
+  <si>
+    <t>NeurIPS 2025 OpenReview Conference</t>
+  </si>
+  <si>
+    <t>https://openreview.net/group?id=NeurIPS.cc%2F2025%2FConference</t>
+  </si>
+  <si>
+    <t>Names + affiliations + linked profiles</t>
+  </si>
+  <si>
+    <t>Enumerate people lists; resolve to GH (Verified URLs)</t>
+  </si>
+  <si>
+    <t>NeurIPS 2025 OpenReview Workshops</t>
+  </si>
+  <si>
+    <t>https://openreview.net/group?id=NeurIPS.cc%2F2025%2FWorkshop</t>
+  </si>
+  <si>
+    <t>NeurIPS 2025 OpenReview Datasets &amp; Benchmarks</t>
+  </si>
+  <si>
+    <t>https://openreview.net/group?id=NeurIPS.cc%2F2025%2FDatasets_and_Benchmarks_Track</t>
+  </si>
+  <si>
+    <t>ICLR 2026 Committees</t>
+  </si>
+  <si>
+    <t>https://iclr.cc/Conferences/2026/Committees</t>
+  </si>
+  <si>
+    <t>ICLR 2026 OpenReview Conference</t>
+  </si>
+  <si>
+    <t>https://openreview.net/group?id=ICLR.cc%2F2026%2FConference</t>
+  </si>
+  <si>
+    <t>ICML 2026 Committees</t>
+  </si>
+  <si>
+    <t>https://icml.cc/Conferences/2026/Committees</t>
+  </si>
+  <si>
+    <t>NeurIPS 2025 OpenReview Root Group</t>
+  </si>
+  <si>
+    <t>https://openreview.net/group?id=NeurIPS.cc%2F2025</t>
+  </si>
+  <si>
+    <t>Root group catch-all</t>
   </si>
 </sst>
 </file>
@@ -2146,7 +2200,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -2159,7 +2213,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2181,14 +2235,15 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2511,7 +2566,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="MASTERSEEDHUBSTbl" displayName="MASTERSEEDHUBSTbl" ref="A1:K96">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="MASTERSEEDHUBSTbl" displayName="MASTERSEEDHUBSTbl" ref="A1:K103">
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Tier"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Category"/>
@@ -14596,18 +14651,18 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:Q12"/>
+  <dimension ref="A1:Q19"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" zoomScale="137" zoomScaleNormal="137" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="137" zoomScaleNormal="137" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I34" sqref="I34"/>
+      <selection pane="bottomLeft" activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17.5" customWidth="1"/>
     <col min="2" max="2" width="28" customWidth="1"/>
-    <col min="3" max="3" width="18.6640625" customWidth="1"/>
+    <col min="3" max="3" width="33.83203125" customWidth="1"/>
     <col min="4" max="4" width="26.1640625" customWidth="1"/>
     <col min="5" max="5" width="28" customWidth="1"/>
     <col min="6" max="6" width="34.83203125" customWidth="1"/>
@@ -14676,422 +14731,778 @@
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="18" t="s">
         <v>75</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="18" t="s">
         <v>76</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="18" t="s">
         <v>77</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="18" t="s">
         <v>78</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="18" t="s">
         <v>79</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="18" t="s">
         <v>80</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="18" t="s">
         <v>81</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="18" t="s">
         <v>82</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="I2" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="J2" s="18" t="s">
         <v>84</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="K2" s="18" t="s">
         <v>85</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="L2" s="18" t="s">
         <v>9</v>
       </c>
+      <c r="M2" s="17"/>
+      <c r="N2" s="17"/>
+      <c r="O2" s="17"/>
+      <c r="P2" s="17"/>
+      <c r="Q2" s="17"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="A3" s="18" t="s">
         <v>75</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="18" t="s">
         <v>76</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="18" t="s">
         <v>77</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="18" t="s">
         <v>78</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="18" t="s">
         <v>79</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="18" t="s">
         <v>86</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" s="18" t="s">
         <v>81</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" s="18" t="s">
         <v>82</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I3" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="J3" t="s">
+      <c r="J3" s="18" t="s">
         <v>84</v>
       </c>
-      <c r="K3" t="s">
+      <c r="K3" s="18" t="s">
         <v>85</v>
       </c>
-      <c r="L3" t="s">
+      <c r="L3" s="18" t="s">
         <v>9</v>
       </c>
+      <c r="M3" s="17"/>
+      <c r="N3" s="17"/>
+      <c r="O3" s="17"/>
+      <c r="P3" s="17"/>
+      <c r="Q3" s="17"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="18" t="s">
         <v>75</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="18" t="s">
         <v>76</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="18" t="s">
         <v>77</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="18" t="s">
         <v>78</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="18" t="s">
         <v>79</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" s="18" t="s">
         <v>87</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="G4" s="18" t="s">
         <v>81</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="H4" s="18" t="s">
         <v>82</v>
       </c>
-      <c r="I4" s="3" t="s">
+      <c r="I4" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="J4" s="3" t="s">
+      <c r="J4" s="18" t="s">
         <v>84</v>
       </c>
-      <c r="K4" s="3" t="s">
+      <c r="K4" s="18" t="s">
         <v>85</v>
       </c>
-      <c r="L4" s="3" t="s">
+      <c r="L4" s="18" t="s">
         <v>9</v>
       </c>
+      <c r="M4" s="17"/>
+      <c r="N4" s="17"/>
+      <c r="O4" s="17"/>
+      <c r="P4" s="17"/>
+      <c r="Q4" s="17"/>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="A5" s="18" t="s">
         <v>75</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="18" t="s">
         <v>76</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="18" t="s">
         <v>88</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="18" t="s">
         <v>89</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="18" t="s">
         <v>90</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" s="18" t="s">
         <v>91</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G5" s="18" t="s">
         <v>81</v>
       </c>
-      <c r="H5" t="s">
+      <c r="H5" s="18" t="s">
         <v>82</v>
       </c>
-      <c r="I5" t="s">
+      <c r="I5" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="J5" t="s">
+      <c r="J5" s="18" t="s">
         <v>84</v>
       </c>
-      <c r="K5" t="s">
+      <c r="K5" s="18" t="s">
         <v>85</v>
       </c>
-      <c r="L5" t="s">
+      <c r="L5" s="18" t="s">
         <v>9</v>
       </c>
+      <c r="M5" s="17"/>
+      <c r="N5" s="17"/>
+      <c r="O5" s="17"/>
+      <c r="P5" s="17"/>
+      <c r="Q5" s="17"/>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="18" t="s">
         <v>75</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="18" t="s">
         <v>76</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="18" t="s">
         <v>88</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="18" t="s">
         <v>89</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="E6" s="18" t="s">
         <v>90</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="F6" s="18" t="s">
         <v>92</v>
       </c>
-      <c r="G6" s="3" t="s">
+      <c r="G6" s="18" t="s">
         <v>81</v>
       </c>
-      <c r="H6" s="3" t="s">
+      <c r="H6" s="18" t="s">
         <v>82</v>
       </c>
-      <c r="I6" s="3" t="s">
+      <c r="I6" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="J6" s="3" t="s">
+      <c r="J6" s="18" t="s">
         <v>84</v>
       </c>
-      <c r="K6" s="3" t="s">
+      <c r="K6" s="18" t="s">
         <v>85</v>
       </c>
-      <c r="L6" s="3" t="s">
+      <c r="L6" s="18" t="s">
         <v>9</v>
       </c>
+      <c r="M6" s="17"/>
+      <c r="N6" s="17"/>
+      <c r="O6" s="17"/>
+      <c r="P6" s="17"/>
+      <c r="Q6" s="17"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+      <c r="A7" s="18" t="s">
         <v>75</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="18" t="s">
         <v>76</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="18" t="s">
         <v>88</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="18" t="s">
         <v>89</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="18" t="s">
         <v>90</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F7" s="18" t="s">
         <v>93</v>
       </c>
-      <c r="G7" t="s">
+      <c r="G7" s="18" t="s">
         <v>81</v>
       </c>
-      <c r="H7" t="s">
+      <c r="H7" s="18" t="s">
         <v>82</v>
       </c>
-      <c r="I7" t="s">
+      <c r="I7" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="J7" t="s">
+      <c r="J7" s="18" t="s">
         <v>84</v>
       </c>
-      <c r="K7" t="s">
+      <c r="K7" s="18" t="s">
         <v>85</v>
       </c>
-      <c r="L7" t="s">
+      <c r="L7" s="18" t="s">
         <v>9</v>
       </c>
+      <c r="M7" s="17"/>
+      <c r="N7" s="17"/>
+      <c r="O7" s="17"/>
+      <c r="P7" s="17"/>
+      <c r="Q7" s="17"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="18" t="s">
         <v>75</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="18" t="s">
         <v>76</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="18" t="s">
         <v>95</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="E8" s="18" t="s">
         <v>96</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="F8" s="18" t="s">
         <v>97</v>
       </c>
-      <c r="G8" s="3" t="s">
+      <c r="G8" s="18" t="s">
         <v>81</v>
       </c>
-      <c r="H8" s="3" t="s">
+      <c r="H8" s="18" t="s">
         <v>82</v>
       </c>
-      <c r="I8" s="3" t="s">
+      <c r="I8" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="J8" s="3" t="s">
+      <c r="J8" s="18" t="s">
         <v>84</v>
       </c>
-      <c r="K8" s="3" t="s">
+      <c r="K8" s="18" t="s">
         <v>85</v>
       </c>
-      <c r="L8" s="3" t="s">
+      <c r="L8" s="18" t="s">
         <v>9</v>
       </c>
+      <c r="M8" s="17"/>
+      <c r="N8" s="17"/>
+      <c r="O8" s="17"/>
+      <c r="P8" s="17"/>
+      <c r="Q8" s="17"/>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+      <c r="A9" s="18" t="s">
         <v>75</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="18" t="s">
         <v>76</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="18" t="s">
         <v>95</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="18" t="s">
         <v>96</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F9" s="18" t="s">
         <v>98</v>
       </c>
-      <c r="G9" t="s">
+      <c r="G9" s="18" t="s">
         <v>81</v>
       </c>
-      <c r="H9" t="s">
+      <c r="H9" s="18" t="s">
         <v>82</v>
       </c>
-      <c r="I9" t="s">
+      <c r="I9" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="J9" t="s">
+      <c r="J9" s="18" t="s">
         <v>84</v>
       </c>
-      <c r="K9" t="s">
+      <c r="K9" s="18" t="s">
         <v>85</v>
       </c>
-      <c r="L9" t="s">
+      <c r="L9" s="18" t="s">
         <v>9</v>
       </c>
+      <c r="M9" s="17"/>
+      <c r="N9" s="17"/>
+      <c r="O9" s="17"/>
+      <c r="P9" s="17"/>
+      <c r="Q9" s="17"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="18" t="s">
         <v>75</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="18" t="s">
         <v>76</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D10" s="18" t="s">
         <v>95</v>
       </c>
-      <c r="E10" s="3" t="s">
+      <c r="E10" s="18" t="s">
         <v>96</v>
       </c>
-      <c r="F10" s="3" t="s">
+      <c r="F10" s="18" t="s">
         <v>99</v>
       </c>
-      <c r="G10" s="3" t="s">
+      <c r="G10" s="18" t="s">
         <v>81</v>
       </c>
-      <c r="H10" s="3" t="s">
+      <c r="H10" s="18" t="s">
         <v>82</v>
       </c>
-      <c r="I10" s="3" t="s">
+      <c r="I10" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="J10" s="3" t="s">
+      <c r="J10" s="18" t="s">
         <v>84</v>
       </c>
-      <c r="K10" s="3" t="s">
+      <c r="K10" s="18" t="s">
         <v>85</v>
       </c>
-      <c r="L10" s="3" t="s">
+      <c r="L10" s="18" t="s">
         <v>9</v>
       </c>
+      <c r="M10" s="17"/>
+      <c r="N10" s="17"/>
+      <c r="O10" s="17"/>
+      <c r="P10" s="17"/>
+      <c r="Q10" s="17"/>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+      <c r="A11" s="18" t="s">
         <v>75</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="18" t="s">
         <v>76</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="18" t="s">
         <v>95</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" s="18" t="s">
         <v>100</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F11" s="18" t="s">
         <v>101</v>
       </c>
-      <c r="G11" t="s">
+      <c r="G11" s="18" t="s">
         <v>81</v>
       </c>
-      <c r="H11" t="s">
+      <c r="H11" s="18" t="s">
         <v>82</v>
       </c>
-      <c r="I11" t="s">
+      <c r="I11" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="J11" t="s">
+      <c r="J11" s="18" t="s">
         <v>84</v>
       </c>
-      <c r="K11" t="s">
+      <c r="K11" s="18" t="s">
         <v>85</v>
       </c>
-      <c r="L11" t="s">
+      <c r="L11" s="18" t="s">
         <v>9</v>
       </c>
+      <c r="M11" s="17"/>
+      <c r="N11" s="17"/>
+      <c r="O11" s="17"/>
+      <c r="P11" s="17"/>
+      <c r="Q11" s="17"/>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="18" t="s">
         <v>75</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="18" t="s">
         <v>76</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="18" t="s">
         <v>88</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="D12" s="18" t="s">
         <v>89</v>
       </c>
-      <c r="E12" s="3" t="s">
+      <c r="E12" s="18" t="s">
         <v>102</v>
       </c>
-      <c r="F12" s="3" t="s">
+      <c r="F12" s="18" t="s">
         <v>103</v>
       </c>
-      <c r="G12" s="3" t="s">
+      <c r="G12" s="18" t="s">
         <v>81</v>
       </c>
-      <c r="H12" s="3" t="s">
+      <c r="H12" s="18" t="s">
         <v>82</v>
       </c>
-      <c r="I12" s="3" t="s">
+      <c r="I12" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="J12" s="3" t="s">
+      <c r="J12" s="18" t="s">
         <v>84</v>
       </c>
-      <c r="K12" s="3" t="s">
+      <c r="K12" s="18" t="s">
         <v>85</v>
       </c>
-      <c r="L12" s="3" t="s">
+      <c r="L12" s="18" t="s">
         <v>9</v>
       </c>
+      <c r="M12" s="17"/>
+      <c r="N12" s="17"/>
+      <c r="O12" s="17"/>
+      <c r="P12" s="17"/>
+      <c r="Q12" s="17"/>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A13" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="B13" s="18" t="s">
+        <v>76</v>
+      </c>
+      <c r="C13" s="18" t="s">
+        <v>657</v>
+      </c>
+      <c r="D13" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="E13" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="F13" s="18" t="s">
+        <v>658</v>
+      </c>
+      <c r="G13" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="H13" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="I13" s="18" t="s">
+        <v>659</v>
+      </c>
+      <c r="J13" s="18" t="s">
+        <v>660</v>
+      </c>
+      <c r="K13" s="18" t="s">
+        <v>113</v>
+      </c>
+      <c r="L13" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="M13" s="17"/>
+      <c r="N13" s="17"/>
+      <c r="O13" s="17"/>
+      <c r="P13" s="17"/>
+      <c r="Q13" s="17"/>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A14" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="B14" s="18" t="s">
+        <v>76</v>
+      </c>
+      <c r="C14" s="18" t="s">
+        <v>661</v>
+      </c>
+      <c r="D14" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="E14" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="F14" s="18" t="s">
+        <v>662</v>
+      </c>
+      <c r="G14" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="H14" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="I14" s="18" t="s">
+        <v>659</v>
+      </c>
+      <c r="J14" s="18" t="s">
+        <v>660</v>
+      </c>
+      <c r="K14" s="18" t="s">
+        <v>113</v>
+      </c>
+      <c r="L14" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="M14" s="17"/>
+      <c r="N14" s="17"/>
+      <c r="O14" s="17"/>
+      <c r="P14" s="17"/>
+      <c r="Q14" s="17"/>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A15" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="B15" s="18" t="s">
+        <v>76</v>
+      </c>
+      <c r="C15" s="18" t="s">
+        <v>663</v>
+      </c>
+      <c r="D15" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="E15" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="F15" s="18" t="s">
+        <v>664</v>
+      </c>
+      <c r="G15" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="H15" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="I15" s="18" t="s">
+        <v>659</v>
+      </c>
+      <c r="J15" s="18" t="s">
+        <v>660</v>
+      </c>
+      <c r="K15" s="18" t="s">
+        <v>113</v>
+      </c>
+      <c r="L15" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="M15" s="17"/>
+      <c r="N15" s="17"/>
+      <c r="O15" s="17"/>
+      <c r="P15" s="17"/>
+      <c r="Q15" s="17"/>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A16" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="B16" s="18" t="s">
+        <v>76</v>
+      </c>
+      <c r="C16" s="18" t="s">
+        <v>671</v>
+      </c>
+      <c r="D16" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="E16" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="F16" s="18" t="s">
+        <v>672</v>
+      </c>
+      <c r="G16" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="H16" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="I16" s="18" t="s">
+        <v>659</v>
+      </c>
+      <c r="J16" s="18" t="s">
+        <v>673</v>
+      </c>
+      <c r="K16" s="18" t="s">
+        <v>113</v>
+      </c>
+      <c r="L16" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="M16" s="17"/>
+      <c r="N16" s="17"/>
+      <c r="O16" s="17"/>
+      <c r="P16" s="17"/>
+      <c r="Q16" s="17"/>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A17" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="B17" s="18" t="s">
+        <v>76</v>
+      </c>
+      <c r="C17" s="18" t="s">
+        <v>665</v>
+      </c>
+      <c r="D17" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="E17" s="18" t="s">
+        <v>102</v>
+      </c>
+      <c r="F17" s="18" t="s">
+        <v>666</v>
+      </c>
+      <c r="G17" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="H17" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="I17" s="18" t="s">
+        <v>659</v>
+      </c>
+      <c r="J17" s="18" t="s">
+        <v>660</v>
+      </c>
+      <c r="K17" s="18" t="s">
+        <v>113</v>
+      </c>
+      <c r="L17" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="M17" s="17"/>
+      <c r="N17" s="17"/>
+      <c r="O17" s="17"/>
+      <c r="P17" s="17"/>
+      <c r="Q17" s="17"/>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A18" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="B18" s="18" t="s">
+        <v>76</v>
+      </c>
+      <c r="C18" s="18" t="s">
+        <v>667</v>
+      </c>
+      <c r="D18" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="E18" s="18" t="s">
+        <v>102</v>
+      </c>
+      <c r="F18" s="18" t="s">
+        <v>668</v>
+      </c>
+      <c r="G18" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="H18" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="I18" s="18" t="s">
+        <v>659</v>
+      </c>
+      <c r="J18" s="18" t="s">
+        <v>660</v>
+      </c>
+      <c r="K18" s="18" t="s">
+        <v>113</v>
+      </c>
+      <c r="L18" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="M18" s="17"/>
+      <c r="N18" s="17"/>
+      <c r="O18" s="17"/>
+      <c r="P18" s="17"/>
+      <c r="Q18" s="17"/>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A19" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="B19" s="18" t="s">
+        <v>76</v>
+      </c>
+      <c r="C19" s="18" t="s">
+        <v>669</v>
+      </c>
+      <c r="D19" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="E19" s="18" t="s">
+        <v>100</v>
+      </c>
+      <c r="F19" s="18" t="s">
+        <v>670</v>
+      </c>
+      <c r="G19" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="H19" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="I19" s="18" t="s">
+        <v>659</v>
+      </c>
+      <c r="J19" s="18" t="s">
+        <v>660</v>
+      </c>
+      <c r="K19" s="18" t="s">
+        <v>113</v>
+      </c>
+      <c r="L19" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="M19" s="17"/>
+      <c r="N19" s="17"/>
+      <c r="O19" s="17"/>
+      <c r="P19" s="17"/>
+      <c r="Q19" s="17"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -15102,7 +15513,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:Q21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="163" zoomScaleNormal="163" workbookViewId="0">
+    <sheetView zoomScale="163" zoomScaleNormal="163" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B20" sqref="B20"/>
     </sheetView>
@@ -16493,16 +16904,24 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:P96"/>
+  <dimension ref="A1:Q103"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="132" zoomScaleNormal="132" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A49" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M62" sqref="M53:M62"/>
+    <sheetView zoomScale="132" zoomScaleNormal="132" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A58" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A97" sqref="A97:XFD103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="11" width="28" customWidth="1"/>
+    <col min="1" max="1" width="18.33203125" customWidth="1"/>
+    <col min="2" max="2" width="28" customWidth="1"/>
+    <col min="3" max="3" width="34.83203125" customWidth="1"/>
+    <col min="4" max="4" width="24.33203125" customWidth="1"/>
+    <col min="5" max="5" width="28" customWidth="1"/>
+    <col min="6" max="6" width="72.6640625" customWidth="1"/>
+    <col min="7" max="7" width="31.5" customWidth="1"/>
+    <col min="8" max="10" width="28" customWidth="1"/>
+    <col min="11" max="11" width="18.5" customWidth="1"/>
     <col min="12" max="12" width="13.1640625" customWidth="1"/>
     <col min="13" max="13" width="15.1640625" customWidth="1"/>
     <col min="14" max="14" width="13.1640625" customWidth="1"/>
@@ -18440,7 +18859,7 @@
       <c r="O48" s="16"/>
       <c r="P48" s="16"/>
     </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>267</v>
       </c>
@@ -18480,7 +18899,7 @@
       <c r="O49" s="6"/>
       <c r="P49" s="6"/>
     </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A50" s="3" t="s">
         <v>267</v>
       </c>
@@ -18520,7 +18939,7 @@
       <c r="O50" s="16"/>
       <c r="P50" s="16"/>
     </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>267</v>
       </c>
@@ -18560,7 +18979,7 @@
       <c r="O51" s="6"/>
       <c r="P51" s="6"/>
     </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A52" s="3" t="s">
         <v>267</v>
       </c>
@@ -18600,7 +19019,7 @@
       <c r="O52" s="16"/>
       <c r="P52" s="16"/>
     </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>267</v>
       </c>
@@ -18639,8 +19058,11 @@
       <c r="N53" s="6"/>
       <c r="O53" s="6"/>
       <c r="P53" s="6"/>
-    </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q53" t="s">
+        <v>656</v>
+      </c>
+    </row>
+    <row r="54" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A54" s="3" t="s">
         <v>267</v>
       </c>
@@ -18680,7 +19102,7 @@
       <c r="O54" s="16"/>
       <c r="P54" s="16"/>
     </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>267</v>
       </c>
@@ -18720,7 +19142,7 @@
       <c r="O55" s="6"/>
       <c r="P55" s="6"/>
     </row>
-    <row r="56" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A56" s="3" t="s">
         <v>267</v>
       </c>
@@ -18760,7 +19182,7 @@
       <c r="O56" s="16"/>
       <c r="P56" s="16"/>
     </row>
-    <row r="57" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>267</v>
       </c>
@@ -18800,7 +19222,7 @@
       <c r="O57" s="6"/>
       <c r="P57" s="6"/>
     </row>
-    <row r="58" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A58" s="3" t="s">
         <v>201</v>
       </c>
@@ -18840,7 +19262,7 @@
       <c r="O58" s="16"/>
       <c r="P58" s="16"/>
     </row>
-    <row r="59" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>267</v>
       </c>
@@ -18880,7 +19302,7 @@
       <c r="O59" s="6"/>
       <c r="P59" s="6"/>
     </row>
-    <row r="60" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A60" s="3" t="s">
         <v>267</v>
       </c>
@@ -18920,7 +19342,7 @@
       <c r="O60" s="16"/>
       <c r="P60" s="16"/>
     </row>
-    <row r="61" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>267</v>
       </c>
@@ -18960,7 +19382,7 @@
       <c r="O61" s="6"/>
       <c r="P61" s="6"/>
     </row>
-    <row r="62" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A62" s="3" t="s">
         <v>267</v>
       </c>
@@ -19000,7 +19422,7 @@
       <c r="O62" s="16"/>
       <c r="P62" s="16"/>
     </row>
-    <row r="63" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>75</v>
       </c>
@@ -19040,7 +19462,7 @@
       <c r="O63" s="6"/>
       <c r="P63" s="6"/>
     </row>
-    <row r="64" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A64" s="3" t="s">
         <v>75</v>
       </c>
@@ -20359,6 +20781,286 @@
       <c r="N96" s="17"/>
       <c r="O96" s="17"/>
       <c r="P96" s="17"/>
+    </row>
+    <row r="97" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A97" t="s">
+        <v>75</v>
+      </c>
+      <c r="B97" t="s">
+        <v>76</v>
+      </c>
+      <c r="C97" t="s">
+        <v>657</v>
+      </c>
+      <c r="D97" t="s">
+        <v>78</v>
+      </c>
+      <c r="E97" t="s">
+        <v>79</v>
+      </c>
+      <c r="F97" t="s">
+        <v>658</v>
+      </c>
+      <c r="G97" t="s">
+        <v>81</v>
+      </c>
+      <c r="H97" t="s">
+        <v>82</v>
+      </c>
+      <c r="I97" t="s">
+        <v>659</v>
+      </c>
+      <c r="J97" t="s">
+        <v>660</v>
+      </c>
+      <c r="K97" t="s">
+        <v>113</v>
+      </c>
+      <c r="L97" s="17"/>
+      <c r="M97" s="17"/>
+      <c r="N97" s="17"/>
+      <c r="O97" s="17"/>
+      <c r="P97" s="17"/>
+    </row>
+    <row r="98" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A98" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="B98" s="18" t="s">
+        <v>76</v>
+      </c>
+      <c r="C98" s="18" t="s">
+        <v>661</v>
+      </c>
+      <c r="D98" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="E98" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="F98" s="18" t="s">
+        <v>662</v>
+      </c>
+      <c r="G98" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="H98" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="I98" s="18" t="s">
+        <v>659</v>
+      </c>
+      <c r="J98" s="18" t="s">
+        <v>660</v>
+      </c>
+      <c r="K98" s="18" t="s">
+        <v>113</v>
+      </c>
+      <c r="L98" s="17"/>
+      <c r="M98" s="17"/>
+      <c r="N98" s="17"/>
+      <c r="O98" s="17"/>
+      <c r="P98" s="17"/>
+    </row>
+    <row r="99" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A99" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="B99" s="18" t="s">
+        <v>76</v>
+      </c>
+      <c r="C99" s="18" t="s">
+        <v>663</v>
+      </c>
+      <c r="D99" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="E99" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="F99" s="18" t="s">
+        <v>664</v>
+      </c>
+      <c r="G99" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="H99" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="I99" s="18" t="s">
+        <v>659</v>
+      </c>
+      <c r="J99" s="18" t="s">
+        <v>660</v>
+      </c>
+      <c r="K99" s="18" t="s">
+        <v>113</v>
+      </c>
+      <c r="L99" s="17"/>
+      <c r="M99" s="17"/>
+      <c r="N99" s="17"/>
+      <c r="O99" s="17"/>
+      <c r="P99" s="17"/>
+    </row>
+    <row r="100" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A100" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="B100" s="18" t="s">
+        <v>76</v>
+      </c>
+      <c r="C100" s="18" t="s">
+        <v>671</v>
+      </c>
+      <c r="D100" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="E100" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="F100" s="18" t="s">
+        <v>672</v>
+      </c>
+      <c r="G100" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="H100" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="I100" s="18" t="s">
+        <v>659</v>
+      </c>
+      <c r="J100" s="18" t="s">
+        <v>673</v>
+      </c>
+      <c r="K100" s="18" t="s">
+        <v>113</v>
+      </c>
+      <c r="L100" s="17"/>
+      <c r="M100" s="17"/>
+      <c r="N100" s="17"/>
+      <c r="O100" s="17"/>
+      <c r="P100" s="17"/>
+    </row>
+    <row r="101" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A101" t="s">
+        <v>75</v>
+      </c>
+      <c r="B101" t="s">
+        <v>76</v>
+      </c>
+      <c r="C101" t="s">
+        <v>665</v>
+      </c>
+      <c r="D101" t="s">
+        <v>89</v>
+      </c>
+      <c r="E101" t="s">
+        <v>102</v>
+      </c>
+      <c r="F101" t="s">
+        <v>666</v>
+      </c>
+      <c r="G101" t="s">
+        <v>81</v>
+      </c>
+      <c r="H101" t="s">
+        <v>82</v>
+      </c>
+      <c r="I101" t="s">
+        <v>659</v>
+      </c>
+      <c r="J101" t="s">
+        <v>660</v>
+      </c>
+      <c r="K101" t="s">
+        <v>113</v>
+      </c>
+      <c r="L101" s="17"/>
+      <c r="M101" s="17"/>
+      <c r="N101" s="17"/>
+      <c r="O101" s="17"/>
+      <c r="P101" s="17"/>
+    </row>
+    <row r="102" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A102" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="B102" s="18" t="s">
+        <v>76</v>
+      </c>
+      <c r="C102" s="18" t="s">
+        <v>667</v>
+      </c>
+      <c r="D102" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="E102" s="18" t="s">
+        <v>102</v>
+      </c>
+      <c r="F102" s="18" t="s">
+        <v>668</v>
+      </c>
+      <c r="G102" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="H102" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="I102" s="18" t="s">
+        <v>659</v>
+      </c>
+      <c r="J102" s="18" t="s">
+        <v>660</v>
+      </c>
+      <c r="K102" s="18" t="s">
+        <v>113</v>
+      </c>
+      <c r="L102" s="17"/>
+      <c r="M102" s="17"/>
+      <c r="N102" s="17"/>
+      <c r="O102" s="17"/>
+      <c r="P102" s="17"/>
+    </row>
+    <row r="103" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A103" t="s">
+        <v>75</v>
+      </c>
+      <c r="B103" t="s">
+        <v>76</v>
+      </c>
+      <c r="C103" t="s">
+        <v>669</v>
+      </c>
+      <c r="D103" t="s">
+        <v>95</v>
+      </c>
+      <c r="E103" t="s">
+        <v>100</v>
+      </c>
+      <c r="F103" t="s">
+        <v>670</v>
+      </c>
+      <c r="G103" t="s">
+        <v>81</v>
+      </c>
+      <c r="H103" t="s">
+        <v>82</v>
+      </c>
+      <c r="I103" t="s">
+        <v>659</v>
+      </c>
+      <c r="J103" t="s">
+        <v>660</v>
+      </c>
+      <c r="K103" t="s">
+        <v>113</v>
+      </c>
+      <c r="L103" s="17"/>
+      <c r="M103" s="17"/>
+      <c r="N103" s="17"/>
+      <c r="O103" s="17"/>
+      <c r="P103" s="17"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>